<commit_message>
logs and failed tranaction status set
</commit_message>
<xml_diff>
--- a/SportsInviter/Data/Input/LazzyLADS/PlayerDetails.xlsx
+++ b/SportsInviter/Data/Input/LazzyLADS/PlayerDetails.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E5444F-8968-497A-9476-BD700AD2C96B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7508B993-EA94-4836-BD37-CA0940EB2DAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>6410 Breeze Bay Pt, Fort Worth 76131</t>
+  </si>
+  <si>
+    <t>aruncyclopse007@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -555,7 +558,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +605,9 @@
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>38</v>
       </c>
@@ -731,8 +736,9 @@
     <hyperlink ref="B12" r:id="rId10" xr:uid="{A6C287D4-CD42-4934-9060-24CB83EEE46C}"/>
     <hyperlink ref="B13" r:id="rId11" xr:uid="{29C8B4D8-B9D9-4A28-A904-321A3348D344}"/>
     <hyperlink ref="B11" r:id="rId12" xr:uid="{05936C3F-B44B-412F-8904-FBDFA707B410}"/>
+    <hyperlink ref="B4" r:id="rId13" xr:uid="{0EBBBEB6-E7AA-4B45-87E9-665300E9DEE9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>